<commit_message>
python check operatable 11
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmo\Desktop\os2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02A64C9-BBC4-4140-9C77-8B74F3B88362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40C886C-95E9-4766-BC38-430E4445ED70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3795" yWindow="1095" windowWidth="19710" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>احمد</t>
   </si>
   <si>
-    <t xml:space="preserve">   العنوان</t>
-  </si>
-  <si>
     <t>الاسم</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>دمياط</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
 </sst>
 </file>
@@ -369,17 +369,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -387,7 +387,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -395,7 +395,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -403,7 +403,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>